<commit_message>
Add 'Taking Away' sample / end to end test
This exercises multiple worksheets per workbook
</commit_message>
<xml_diff>
--- a/SampleTests/ExcelTests/Calculator.xlsx
+++ b/SampleTests/ExcelTests/Calculator.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cburge\Documents\repos\customer-tests-excel\SampleTests\ExcelTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{56A0E947-76BC-4A1F-A040-DB43C44407D3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{64C4F854-328F-4FA2-A1EF-85C991532800}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{93574C7F-CD34-4A26-A791-2CAAC18DAAC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Adding Up" sheetId="1" r:id="rId1"/>
+    <sheet name="Taking Away" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Specification</t>
   </si>
@@ -79,15 +80,33 @@
   </si>
   <si>
     <t>Leading, trailing and enclosed spaces (leading and trailing spaces are ignored, enclosed spaces are converted to underscores)</t>
+  </si>
+  <si>
+    <t>Operation.Subtract</t>
+  </si>
+  <si>
+    <t>Calculator</t>
+  </si>
+  <si>
+    <t>FirstValue of</t>
+  </si>
+  <si>
+    <t>Perform Operation</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Multiple worksheets per workbook</t>
+  </si>
+  <si>
+    <t>PercentagePrecision</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -122,14 +141,220 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -546,7 +771,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,7 +780,7 @@
     <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="16" style="1" customWidth="1"/>
     <col min="7" max="7" width="60" style="1" customWidth="1"/>
     <col min="8" max="8" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -646,50 +871,260 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:XFD11 A13:XFD1048576 A12:D12 G12:XFD12">
+    <cfRule type="cellIs" dxfId="12" priority="17" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="18" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="20" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="8" priority="21" operator="beginsWith" text="With Properties">
+      <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="7" priority="22" operator="endsWith" text=" table of">
+      <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="6" priority="23" operator="endsWith" text=" of">
+      <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="24">
+      <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="25">
+      <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD11 A13:XFD1048576 A12:D12 G12:XFD12">
+    <cfRule type="notContainsBlanks" dxfId="3" priority="26">
+      <formula>LEN(TRIM(A1))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD11 A13:XFD1048576 A12:D12 G12:XFD12">
+    <cfRule type="cellIs" dxfId="2" priority="15" operator="equal">
+      <formula>"PercentagePrecision"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="16" operator="equal">
+      <formula>"="</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:XFD11 A13:XFD1048576 A12:D12 G12:XFD12">
+    <cfRule type="cellIs" dxfId="0" priority="14" operator="equal">
+      <formula>"StringFormat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:F12">
+    <cfRule type="cellIs" dxfId="25" priority="4" operator="equal">
+      <formula>"Assert"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="5" operator="equal">
+      <formula>"When"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="equal">
+      <formula>"Given a"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+      <formula>"Specification"</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="21" priority="8" operator="beginsWith" text="With Properties">
+      <formula>LEFT(E12,LEN("With Properties"))="With Properties"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="20" priority="9" operator="endsWith" text=" table of">
+      <formula>RIGHT(E12,LEN(" table of"))=" table of"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="19" priority="10" operator="endsWith" text=" of">
+      <formula>RIGHT(E12,LEN(" of"))=" of"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="11">
+      <formula>AND((RIGHT(E11, 3) = " of"), E13 = "With Properties")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="12">
+      <formula>AND(RIGHT(D12, 3) = " of", E13 = "With Properties")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:F12">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="13">
+      <formula>LEN(TRIM(E12))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:F12">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+      <formula>"PercentagePrecision"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="equal">
+      <formula>"="</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12:F12">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+      <formula>"StringFormat"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07917FFE-3CF1-4F24-ADDD-99FADF944328}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="E12:F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="20" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="1" customWidth="1"/>
+    <col min="7" max="7" width="60" style="1" customWidth="1"/>
+    <col min="8" max="8" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1E-4</v>
+      </c>
+    </row>
+  </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="12" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="equal">
       <formula>"Assert"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="equal">
       <formula>"When"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="equal">
       <formula>"Given a"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="equal">
       <formula>"Specification"</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="8" priority="8" operator="beginsWith" text="With Properties">
+    <cfRule type="beginsWith" dxfId="34" priority="8" operator="beginsWith" text="With Properties">
       <formula>LEFT(A1,LEN("With Properties"))="With Properties"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="7" priority="9" operator="endsWith" text=" table of">
+    <cfRule type="endsWith" dxfId="33" priority="9" operator="endsWith" text=" table of">
       <formula>RIGHT(A1,LEN(" table of"))=" table of"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="6" priority="10" operator="endsWith" text=" of">
+    <cfRule type="endsWith" dxfId="32" priority="10" operator="endsWith" text=" of">
       <formula>RIGHT(A1,LEN(" of"))=" of"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="11">
+    <cfRule type="expression" dxfId="31" priority="11">
       <formula>AND((RIGHT(A1048576, 3) = " of"), A2 = "With Properties")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="12">
+    <cfRule type="expression" dxfId="30" priority="12">
       <formula>AND(RIGHT(XFD1, 3) = " of", A2 = "With Properties")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="notContainsBlanks" dxfId="3" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="13">
       <formula>LEN(TRIM(A1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="equal">
       <formula>"PercentagePrecision"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="equal">
       <formula>"="</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
       <formula>"StringFormat"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>